<commit_message>
Adiciona suporte bilíngue e melhorias visuais no dashboard
</commit_message>
<xml_diff>
--- a/data/ASSAY.xlsx
+++ b/data/ASSAY.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://brminbr-my.sharepoint.com/personal/exim9_brminbr_com/Documents/gestao-sst/6. Empresa de Grande Porte-Large-Sized Enterprise (LSE)/Brasil Minerais-WMA/12. Geologia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\BRAZIL MINERALS\dashboard_manganes_3d\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{1B3B178F-2A5F-456D-B446-F2405B0FE0B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59F4E279-970E-4AE2-BC60-13F6BB72EB6D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AD7E15-FC83-42D4-9111-43392B35D2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="B550" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -2652,204 +2652,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF800080"/>
-          <bgColor rgb="FF800080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFA500"/>
-          <bgColor rgb="FFFFA500"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0000FF"/>
-          <bgColor rgb="FF0000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF800080"/>
-          <bgColor rgb="FF800080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFA500"/>
-          <bgColor rgb="FFFFA500"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0000FF"/>
-          <bgColor rgb="FF0000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF800080"/>
-          <bgColor rgb="FF800080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFA500"/>
-          <bgColor rgb="FFFFA500"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0000FF"/>
-          <bgColor rgb="FF0000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF800080"/>
-          <bgColor rgb="FF800080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFA500"/>
-          <bgColor rgb="FFFFA500"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0000FF"/>
-          <bgColor rgb="FF0000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3249,8 +3059,8 @@
   </sheetPr>
   <dimension ref="A1:AP698"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A538" workbookViewId="0">
-      <selection activeCell="A554" sqref="A554:AL562"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -76567,132 +76377,28 @@
     </row>
   </sheetData>
   <autoFilter ref="F1:F191" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="F2:F485">
-    <cfRule type="cellIs" dxfId="35" priority="151" operator="between">
+  <conditionalFormatting sqref="F2:F698">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="between">
       <formula>0</formula>
       <formula>10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="152" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="between">
       <formula>10.1</formula>
       <formula>18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="153" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="between">
       <formula>18.01</formula>
       <formula>28</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="154" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="between">
       <formula>28.01</formula>
       <formula>38</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="155" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="between">
       <formula>38.01</formula>
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="156" operator="between">
-      <formula>50.01</formula>
-      <formula>60</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F496:F553">
-    <cfRule type="cellIs" dxfId="29" priority="115" operator="between">
-      <formula>0</formula>
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="116" operator="between">
-      <formula>10.1</formula>
-      <formula>18</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="117" operator="between">
-      <formula>18.01</formula>
-      <formula>28</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="118" operator="between">
-      <formula>28.01</formula>
-      <formula>38</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="119" operator="between">
-      <formula>38.01</formula>
-      <formula>50</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="120" operator="between">
-      <formula>50.01</formula>
-      <formula>60</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F563:F698">
-    <cfRule type="cellIs" dxfId="23" priority="13" operator="between">
-      <formula>0</formula>
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="14" operator="between">
-      <formula>10.1</formula>
-      <formula>18</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="15" operator="between">
-      <formula>18.01</formula>
-      <formula>28</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="16" operator="between">
-      <formula>28.01</formula>
-      <formula>38</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="17" operator="between">
-      <formula>38.01</formula>
-      <formula>50</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="between">
-      <formula>50.01</formula>
-      <formula>60</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F486:F495">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="between">
-      <formula>0</formula>
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="between">
-      <formula>10.1</formula>
-      <formula>18</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="between">
-      <formula>18.01</formula>
-      <formula>28</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="between">
-      <formula>28.01</formula>
-      <formula>38</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="between">
-      <formula>38.01</formula>
-      <formula>50</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="between">
-      <formula>50.01</formula>
-      <formula>60</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F554:F562">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="between">
-      <formula>0</formula>
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
-      <formula>10.1</formula>
-      <formula>18</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="between">
-      <formula>18.01</formula>
-      <formula>28</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="between">
-      <formula>28.01</formula>
-      <formula>38</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="between">
-      <formula>38.01</formula>
-      <formula>50</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="between">
       <formula>50.01</formula>
       <formula>60</formula>
     </cfRule>
@@ -77253,22 +76959,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D38">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>AND($A2="Mn", D2&gt;=0, D2&lt;=10)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>AND($A2="Mn", D2&gt;=10.1, D2&lt;=18)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>AND($A2="Mn", D2&gt;=18.01, D2&lt;=28)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>AND($A2="Mn", D2&gt;=28.01, D2&lt;=38)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>AND($A2="Mn", D2&gt;=38.01, D2&lt;=50)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>AND($A2="Mn", D2&gt;=50.01, D2&lt;=60)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Adiciona aba CUTOFF com filtro interativo e análises inteligentes por localidade
</commit_message>
<xml_diff>
--- a/data/ASSAY.xlsx
+++ b/data/ASSAY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\BRAZIL MINERALS\dashboard_manganes_3d\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AD7E15-FC83-42D4-9111-43392B35D2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD92E20-27B1-4A4B-93E7-B87B4090A554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="B550" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2248" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2248" uniqueCount="849">
   <si>
     <t>Datetime</t>
   </si>
@@ -2586,6 +2586,9 @@
   </si>
   <si>
     <t>18/04/2025 16:13:26</t>
+  </si>
+  <si>
+    <t>MN</t>
   </si>
 </sst>
 </file>
@@ -3060,7 +3063,7 @@
   <dimension ref="A1:AP698"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3089,7 +3092,7 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1</v>
+        <v>848</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>

</xml_diff>